<commit_message>
Update experimental results in table.2
</commit_message>
<xml_diff>
--- a/experiments/MEIT_metric_bigneruon.xlsx
+++ b/experiments/MEIT_metric_bigneruon.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NeuronSeg\Write_Paper\Illustrations\trace_result\BigNeuron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3181AD64-2307-4F96-B523-3D3E27D5BC62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2687C01-C217-48A9-B1A7-94D7EDAF33FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="18820" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="33">
   <si>
     <t>Sample</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +113,38 @@
   </si>
   <si>
     <t>MEIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>best</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GMR_C1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -253,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,12 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -338,13 +370,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -629,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -639,7 +682,7 @@
     <col min="2" max="2" width="11.08203125" style="4" customWidth="1"/>
     <col min="3" max="9" width="8.58203125" style="4"/>
     <col min="10" max="10" width="10.58203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.75" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="4" customWidth="1"/>
     <col min="12" max="12" width="9.83203125" style="4" customWidth="1"/>
     <col min="13" max="16384" width="8.58203125" style="4"/>
   </cols>
@@ -664,21 +707,21 @@
       <c r="AL1" s="5"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="24"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
       <c r="AG2" s="5"/>
       <c r="AH2" s="5"/>
       <c r="AI2" s="5"/>
@@ -687,6 +730,18 @@
       <c r="AL2" s="5"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="K3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
@@ -714,9 +769,32 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="28"/>
+      <c r="G4" s="26"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="K4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="36"/>
+      <c r="M4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
@@ -735,20 +813,45 @@
       <c r="AK4" s="5"/>
       <c r="AL4" s="5"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:38" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="37" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="40"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="K5" s="28">
+        <v>3</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>50</v>
+      </c>
+      <c r="N5" s="41">
+        <v>0.75821428571428495</v>
+      </c>
+      <c r="O5" s="20">
+        <v>0.88682295877121997</v>
+      </c>
+      <c r="P5" s="19">
+        <v>0.81749132245336797</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>0.37312925170068001</v>
+      </c>
+      <c r="R5" s="5">
+        <v>2.1778021750514E-2</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -767,9 +870,9 @@
       <c r="AK5" s="5"/>
       <c r="AL5" s="5"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
-      <c r="B6" s="29"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="10">
         <v>10</v>
       </c>
@@ -789,7 +892,32 @@
         <v>20</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="10"/>
+      <c r="K6" s="28">
+        <v>4</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="5">
+        <v>50</v>
+      </c>
+      <c r="N6" s="41">
+        <v>0.89848121502797695</v>
+      </c>
+      <c r="O6" s="20">
+        <v>0.58833619210977695</v>
+      </c>
+      <c r="P6" s="19">
+        <v>0.71106110837018199</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>0.396302715193529</v>
+      </c>
+      <c r="R6" s="5">
+        <v>1.9781453000740402E-2</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
@@ -812,29 +940,54 @@
       <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="30">
         <v>1.7123255806740699E-2</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="30">
         <v>1.7123255806740699E-2</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="41">
         <v>0.33467787114845898</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="41">
         <v>0.66215469613259603</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="34">
         <v>0.75821428571428495</v>
       </c>
       <c r="H7" s="4">
         <v>2.1778021750514E-2</v>
       </c>
       <c r="J7" s="6"/>
-      <c r="K7" s="25"/>
+      <c r="K7" s="28">
+        <v>5</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="5">
+        <v>10</v>
+      </c>
+      <c r="N7" s="35">
+        <v>0.82246847535345802</v>
+      </c>
+      <c r="O7" s="35">
+        <v>0.96220443120461696</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0.88686594456960199</v>
+      </c>
+      <c r="Q7" s="35">
+        <v>0.38892233594220299</v>
+      </c>
+      <c r="R7" s="5">
+        <v>9.7979334098839299E-2</v>
+      </c>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="6"/>
       <c r="X7" s="5"/>
@@ -857,29 +1010,54 @@
       <c r="A8" s="16">
         <v>4</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="30">
         <v>1.256563316532E-2</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="30">
         <v>1.7745100447311899E-2</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="41">
         <v>0.19285102739726001</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="41">
         <v>0.63504968383017102</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="34">
         <v>0.89848121502797695</v>
       </c>
       <c r="H8" s="4">
         <v>1.9781453000740402E-2</v>
       </c>
       <c r="J8" s="6"/>
-      <c r="K8" s="25"/>
+      <c r="K8" s="28">
+        <v>7</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>50</v>
+      </c>
+      <c r="N8" s="41">
+        <v>0.95712630359212003</v>
+      </c>
+      <c r="O8" s="20">
+        <v>0.98744769874476901</v>
+      </c>
+      <c r="P8" s="19">
+        <v>0.97205060311856395</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>0.54315304948216303</v>
+      </c>
+      <c r="R8" s="5">
+        <v>9.0079583522787599E-3</v>
+      </c>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="6"/>
       <c r="X8" s="5"/>
@@ -900,29 +1078,54 @@
       <c r="A9" s="16">
         <v>5</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="30">
         <v>0.82246847535345802</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="30">
         <v>0.82246847535345802</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="41">
         <v>0.82246847535345802</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="41">
         <v>0.82246847535345802</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="34">
         <v>0.82246847535345802</v>
       </c>
       <c r="H9" s="4">
         <v>9.7979334098839299E-2</v>
       </c>
       <c r="J9" s="6"/>
-      <c r="K9" s="25"/>
+      <c r="K9" s="28">
+        <v>16</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="5">
+        <v>30</v>
+      </c>
+      <c r="N9" s="41">
+        <v>0.94875080076873797</v>
+      </c>
+      <c r="O9" s="20">
+        <v>0.97854077253218796</v>
+      </c>
+      <c r="P9" s="19">
+        <v>0.96341555619909802</v>
+      </c>
+      <c r="Q9" s="20">
+        <v>0.57685009487665995</v>
+      </c>
+      <c r="R9" s="5">
+        <v>3.1475102139591801E-2</v>
+      </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="6"/>
       <c r="X9" s="5"/>
@@ -945,29 +1148,54 @@
       <c r="A10" s="16">
         <v>7</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="30">
         <v>0.170978363123236</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="30">
         <v>0.33359145113829902</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="41">
         <v>0.86085150571131797</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="41">
         <v>0.92962962962962903</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="34">
         <v>0.95712630359212003</v>
       </c>
       <c r="H10" s="4">
         <v>9.0079583522787599E-3</v>
       </c>
       <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="K10" s="28">
+        <v>17</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" s="5">
+        <v>40</v>
+      </c>
+      <c r="N10" s="20">
+        <v>0.99121574139142599</v>
+      </c>
+      <c r="O10" s="20">
+        <v>0.98894154818325397</v>
+      </c>
+      <c r="P10" s="19">
+        <v>0.99007733884190396</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>0.65504011161492803</v>
+      </c>
+      <c r="R10" s="5">
+        <v>3.3112127327532999E-2</v>
+      </c>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="6"/>
       <c r="X10" s="5"/>
@@ -990,13 +1218,13 @@
       <c r="A11" s="16">
         <v>16</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="30">
         <v>0.83708517057321796</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="30">
         <v>0.88068646145464402</v>
       </c>
       <c r="E11" s="20">
@@ -1012,7 +1240,32 @@
         <v>3.1475102139591801E-2</v>
       </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="24"/>
+      <c r="K11" s="28">
+        <v>18</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="28">
+        <v>40</v>
+      </c>
+      <c r="N11" s="20">
+        <v>0.90584737363726398</v>
+      </c>
+      <c r="O11" s="20">
+        <v>0.92273307790549097</v>
+      </c>
+      <c r="P11" s="19">
+        <v>0.91421226173966297</v>
+      </c>
+      <c r="Q11" s="20">
+        <v>0.67554932211313701</v>
+      </c>
+      <c r="R11" s="5">
+        <v>2.5805936887865699E-2</v>
+      </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
@@ -1035,13 +1288,13 @@
       <c r="A12" s="16">
         <v>17</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="30">
         <v>0.96182685753237895</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="30">
         <v>0.98614072494669502</v>
       </c>
       <c r="E12" s="20">
@@ -1057,7 +1310,32 @@
         <v>3.3112127327532999E-2</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="24"/>
+      <c r="K12" s="28">
+        <v>19</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="5">
+        <v>30</v>
+      </c>
+      <c r="N12" s="20">
+        <v>0.998081841432225</v>
+      </c>
+      <c r="O12" s="20">
+        <v>0.95316804407713496</v>
+      </c>
+      <c r="P12" s="19">
+        <v>0.97510803069543095</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>0.84803921568627405</v>
+      </c>
+      <c r="R12" s="5">
+        <v>2.4875401697458301E-2</v>
+      </c>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
       <c r="V12" s="5"/>
       <c r="W12" s="6"/>
       <c r="X12" s="5"/>
@@ -1080,13 +1358,13 @@
       <c r="A13" s="16">
         <v>18</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="30">
         <v>0.84728850325379601</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="30">
         <v>0.86352040816326503</v>
       </c>
       <c r="E13" s="20">
@@ -1102,7 +1380,32 @@
         <v>2.5805936887865699E-2</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" s="20"/>
+      <c r="K13" s="28">
+        <v>20</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="5">
+        <v>30</v>
+      </c>
+      <c r="N13" s="20">
+        <v>0.96190476190476104</v>
+      </c>
+      <c r="O13" s="20">
+        <v>0.93854748603351901</v>
+      </c>
+      <c r="P13" s="19">
+        <v>0.95008258909823895</v>
+      </c>
+      <c r="Q13" s="20">
+        <v>0.76018099547511297</v>
+      </c>
+      <c r="R13" s="5">
+        <v>6.10049926849219E-3</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="6"/>
       <c r="X13" s="5"/>
@@ -1125,13 +1428,13 @@
       <c r="A14" s="16">
         <v>19</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="30">
         <v>0.97694704049844205</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="30">
         <v>0.98614775725593595</v>
       </c>
       <c r="E14" s="20">
@@ -1147,7 +1450,32 @@
         <v>2.4875401697458301E-2</v>
       </c>
       <c r="J14" s="6"/>
-      <c r="K14" s="26"/>
+      <c r="K14" s="28">
+        <v>21</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="5">
+        <v>40</v>
+      </c>
+      <c r="N14" s="20">
+        <v>0.96925144921448303</v>
+      </c>
+      <c r="O14" s="20">
+        <v>0.98730158730158701</v>
+      </c>
+      <c r="P14" s="19">
+        <v>0.97819325767708398</v>
+      </c>
+      <c r="Q14" s="20">
+        <v>0.62205183765313699</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.12680174053524601</v>
+      </c>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="6"/>
       <c r="X14" s="5"/>
@@ -1170,13 +1498,13 @@
       <c r="A15" s="16">
         <v>20</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="30">
         <v>0.68814432989690699</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="30">
         <v>0.84328358208955201</v>
       </c>
       <c r="E15" s="20">
@@ -1192,7 +1520,32 @@
         <v>6.10049926849219E-3</v>
       </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="19"/>
+      <c r="K15" s="28">
+        <v>22</v>
+      </c>
+      <c r="L15" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="5">
+        <v>40</v>
+      </c>
+      <c r="N15" s="20">
+        <v>0.96584938704028001</v>
+      </c>
+      <c r="O15" s="20">
+        <v>0.99080459770114904</v>
+      </c>
+      <c r="P15" s="19">
+        <v>0.97816785270064899</v>
+      </c>
+      <c r="Q15" s="20">
+        <v>0.62536273940800902</v>
+      </c>
+      <c r="R15" s="5">
+        <v>3.6296496498445699E-2</v>
+      </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="6"/>
       <c r="X15" s="5"/>
@@ -1215,13 +1568,13 @@
       <c r="A16" s="16">
         <v>21</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="30">
         <v>0.92399476953252702</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="30">
         <v>0.95154414963027401</v>
       </c>
       <c r="E16" s="20">
@@ -1237,7 +1590,32 @@
         <v>0.12680174053524601</v>
       </c>
       <c r="J16" s="6"/>
-      <c r="K16" s="20"/>
+      <c r="K16" s="28">
+        <v>25</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="5">
+        <v>10</v>
+      </c>
+      <c r="N16" s="35">
+        <v>0.63430602319491203</v>
+      </c>
+      <c r="O16" s="35">
+        <v>0.65739910313901295</v>
+      </c>
+      <c r="P16" s="10">
+        <v>0.64564613434259999</v>
+      </c>
+      <c r="Q16" s="35">
+        <v>0.33872458410351203</v>
+      </c>
+      <c r="R16" s="5">
+        <v>5.7536764751762497E-2</v>
+      </c>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
@@ -1260,13 +1638,13 @@
       <c r="A17" s="16">
         <v>22</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="30">
         <v>0.93960546282245805</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="30">
         <v>0.95243793000299104</v>
       </c>
       <c r="E17" s="20">
@@ -1282,7 +1660,32 @@
         <v>3.6296496498445699E-2</v>
       </c>
       <c r="J17" s="6"/>
-      <c r="K17" s="20"/>
+      <c r="K17" s="28">
+        <v>29</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" s="43">
+        <v>30</v>
+      </c>
+      <c r="N17" s="20">
+        <v>0.93030794165316</v>
+      </c>
+      <c r="O17" s="20">
+        <v>0.88618677042801497</v>
+      </c>
+      <c r="P17" s="19">
+        <v>0.90771152245480002</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>0.46290650406504003</v>
+      </c>
+      <c r="R17" s="5">
+        <v>1.7097556811478499E-2</v>
+      </c>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
       <c r="V17" s="5"/>
       <c r="W17" s="6"/>
       <c r="X17" s="5"/>
@@ -1305,13 +1708,13 @@
       <c r="A18" s="16">
         <v>25</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="30">
         <v>0.63430602319491203</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="30">
         <v>0.69560518731988397</v>
       </c>
       <c r="E18" s="20">
@@ -1327,7 +1730,32 @@
         <v>5.7536764751762497E-2</v>
       </c>
       <c r="J18" s="6"/>
-      <c r="K18" s="20"/>
+      <c r="K18" s="28">
+        <v>31</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="5">
+        <v>50</v>
+      </c>
+      <c r="N18" s="20">
+        <v>0.80225390098246896</v>
+      </c>
+      <c r="O18" s="20">
+        <v>0.97648288476613498</v>
+      </c>
+      <c r="P18" s="19">
+        <v>0.8808354443702</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>0.356856378915202</v>
+      </c>
+      <c r="R18" s="5">
+        <v>6.6991737155132805E-2</v>
+      </c>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
       <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
@@ -1361,13 +1789,13 @@
       <c r="A19" s="16">
         <v>29</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="30">
         <v>0.60460322913088205</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="30">
         <v>0.82442748091603002</v>
       </c>
       <c r="E19" s="20">
@@ -1383,7 +1811,32 @@
         <v>1.7097556811478499E-2</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="K19" s="20"/>
+      <c r="K19" s="28">
+        <v>35</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="5">
+        <v>40</v>
+      </c>
+      <c r="N19" s="20">
+        <v>6.2240663900414899E-3</v>
+      </c>
+      <c r="O19" s="20">
+        <v>7.8737010391686596E-2</v>
+      </c>
+      <c r="P19" s="19">
+        <v>1.15362092523911E-2</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>8.0483719410058396E-3</v>
+      </c>
+      <c r="R19" s="5">
+        <v>4.2580027810611099E-2</v>
+      </c>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
@@ -1417,13 +1870,13 @@
       <c r="A20" s="16">
         <v>31</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="30">
         <v>4.9820690215679697E-2</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="30">
         <v>7.59762423069687E-2</v>
       </c>
       <c r="E20" s="20">
@@ -1439,7 +1892,32 @@
         <v>6.6991737155132805E-2</v>
       </c>
       <c r="J20" s="6"/>
-      <c r="K20" s="20"/>
+      <c r="K20" s="28">
+        <v>50</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="5">
+        <v>50</v>
+      </c>
+      <c r="N20" s="20">
+        <v>0.45979207642596198</v>
+      </c>
+      <c r="O20" s="20">
+        <v>0.39010502340883202</v>
+      </c>
+      <c r="P20" s="19">
+        <v>0.42209156560767502</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>0.22474940769090501</v>
+      </c>
+      <c r="R20" s="5">
+        <v>0.282002348237679</v>
+      </c>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
@@ -1473,11 +1951,11 @@
       <c r="A21" s="16">
         <v>35</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20">
         <v>6.2240663900414899E-3</v>
@@ -1489,7 +1967,32 @@
         <v>4.2580027810611099E-2</v>
       </c>
       <c r="J21" s="6"/>
-      <c r="K21" s="20"/>
+      <c r="K21" s="28">
+        <v>52</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="5">
+        <v>30</v>
+      </c>
+      <c r="N21" s="20">
+        <v>0.54823016272437497</v>
+      </c>
+      <c r="O21" s="20">
+        <v>0.84497231648508597</v>
+      </c>
+      <c r="P21" s="19">
+        <v>0.66499926245762198</v>
+      </c>
+      <c r="Q21" s="20">
+        <v>0.36989835809225902</v>
+      </c>
+      <c r="R21" s="5">
+        <v>0.10077749367633</v>
+      </c>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
@@ -1523,11 +2026,11 @@
       <c r="A22" s="16">
         <v>50</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="20">
         <v>0.14930114358322699</v>
       </c>
@@ -1541,7 +2044,16 @@
         <v>0.282002348237679</v>
       </c>
       <c r="J22" s="6"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
@@ -1597,19 +2109,42 @@
         <v>0.10077749367633</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="K23" s="20"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5">
+        <f t="array" ref="N23">SUM(N5:N21*R5:R21)/SUM(R5:R21)</f>
+        <v>0.68953039431610363</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="array" ref="O23">SUM(O5:O21*R5:R21)/SUM(R5:R21)</f>
+        <v>0.72898027393131593</v>
+      </c>
+      <c r="P23" s="5">
+        <f t="array" ref="P23">SUM(P5:P21*R5:R21)/SUM(R5:R21)</f>
+        <v>0.70202774078123953</v>
+      </c>
+      <c r="Q23" s="5">
+        <f t="array" ref="Q23">SUM(Q5:Q21*R5:R21)/SUM(R5:R21)</f>
+        <v>0.39586252017209483</v>
+      </c>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
-      <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="27"/>
-      <c r="AA23" s="27"/>
-      <c r="AB23" s="27"/>
-      <c r="AC23" s="40"/>
-      <c r="AD23" s="40"/>
-      <c r="AE23" s="40"/>
-      <c r="AF23" s="40"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
+      <c r="AA23" s="25"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="37"/>
+      <c r="AD23" s="37"/>
+      <c r="AE23" s="37"/>
+      <c r="AF23" s="37"/>
       <c r="AG23" s="5"/>
       <c r="AH23" s="5"/>
       <c r="AI23" s="5"/>
@@ -1628,14 +2163,22 @@
       <c r="AV23" s="5"/>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="J24" s="6"/>
       <c r="K24" s="20"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
       <c r="W24" s="9"/>
@@ -1667,6 +2210,15 @@
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.3">
       <c r="K25" s="20"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
@@ -1698,6 +2250,15 @@
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.3">
       <c r="K26" s="20"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
@@ -1736,8 +2297,17 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="28"/>
-      <c r="K27" s="20"/>
+      <c r="G27" s="26"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
@@ -1768,18 +2338,27 @@
       <c r="AV27" s="5"/>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="K28" s="20"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="40"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
@@ -1811,7 +2390,7 @@
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
-      <c r="B29" s="29"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="10">
         <v>10</v>
       </c>
@@ -1830,7 +2409,16 @@
       <c r="H29" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="20"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
@@ -1864,13 +2452,13 @@
       <c r="A30" s="16">
         <v>3</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="30">
         <v>0.98868229587712197</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="30">
         <v>0.98868229587712197</v>
       </c>
       <c r="E30" s="20">
@@ -1885,7 +2473,16 @@
       <c r="H30" s="4">
         <v>2.1778021750514E-2</v>
       </c>
-      <c r="K30" s="20"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
@@ -1919,13 +2516,13 @@
       <c r="A31" s="16">
         <v>4</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="30">
         <v>1</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="30">
         <v>1</v>
       </c>
       <c r="E31" s="20">
@@ -1940,7 +2537,16 @@
       <c r="H31" s="4">
         <v>1.9781453000740402E-2</v>
       </c>
-      <c r="K31" s="20"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
@@ -1974,13 +2580,13 @@
       <c r="A32" s="16">
         <v>5</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="30">
         <v>0.96220443120461696</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="30">
         <v>0.96220443120461696</v>
       </c>
       <c r="E32" s="20">
@@ -1995,7 +2601,16 @@
       <c r="H32" s="4">
         <v>9.7979334098839299E-2</v>
       </c>
-      <c r="K32" s="20"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
       <c r="W32" s="6"/>
@@ -2029,13 +2644,13 @@
       <c r="A33" s="16">
         <v>7</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="32">
+      <c r="C33" s="30">
         <v>1</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="30">
         <v>0.993723849372384</v>
       </c>
       <c r="E33" s="20">
@@ -2050,7 +2665,16 @@
       <c r="H33" s="4">
         <v>9.0079583522787599E-3</v>
       </c>
-      <c r="K33" s="6"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
@@ -2084,13 +2708,13 @@
       <c r="A34" s="16">
         <v>16</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="30">
         <v>0.98712446351931304</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="30">
         <v>0.96834763948497804</v>
       </c>
       <c r="E34" s="20">
@@ -2105,7 +2729,16 @@
       <c r="H34" s="4">
         <v>3.1475102139591801E-2</v>
       </c>
-      <c r="K34" s="6"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
@@ -2139,13 +2772,13 @@
       <c r="A35" s="16">
         <v>17</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="30">
         <v>0.98999473407056304</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="30">
         <v>0.99157451290152698</v>
       </c>
       <c r="E35" s="20">
@@ -2160,7 +2793,16 @@
       <c r="H35" s="4">
         <v>3.3112127327532999E-2</v>
       </c>
-      <c r="K35" s="6"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
@@ -2194,13 +2836,13 @@
       <c r="A36" s="16">
         <v>18</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="30">
         <v>0.94316730523627001</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="30">
         <v>0.95019157088122597</v>
       </c>
       <c r="E36" s="20">
@@ -2215,7 +2857,16 @@
       <c r="H36" s="4">
         <v>2.5805936887865699E-2</v>
       </c>
-      <c r="K36" s="6"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
@@ -2249,13 +2900,13 @@
       <c r="A37" s="16">
         <v>19</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="30">
         <v>0.895316804407713</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="30">
         <v>0.91322314049586695</v>
       </c>
       <c r="E37" s="20">
@@ -2270,7 +2921,16 @@
       <c r="H37" s="4">
         <v>2.4875401697458301E-2</v>
       </c>
-      <c r="K37" s="6"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="6"/>
@@ -2304,13 +2964,13 @@
       <c r="A38" s="16">
         <v>20</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C38" s="30">
         <v>0.93016759776536295</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="30">
         <v>0.93296089385474801</v>
       </c>
       <c r="E38" s="20">
@@ -2325,7 +2985,16 @@
       <c r="H38" s="4">
         <v>6.10049926849219E-3</v>
       </c>
-      <c r="K38" s="6"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
       <c r="U38" s="5"/>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
@@ -2359,13 +3028,13 @@
       <c r="A39" s="16">
         <v>21</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="32">
+      <c r="C39" s="30">
         <v>0.95992063492063495</v>
       </c>
-      <c r="D39" s="32">
+      <c r="D39" s="30">
         <v>0.96931216931216901</v>
       </c>
       <c r="E39" s="20">
@@ -2380,7 +3049,16 @@
       <c r="H39" s="4">
         <v>0.12680174053524601</v>
       </c>
-      <c r="K39" s="6"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
       <c r="W39" s="6"/>
@@ -2414,13 +3092,13 @@
       <c r="A40" s="16">
         <v>22</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="32">
+      <c r="C40" s="30">
         <v>0.96965517241379295</v>
       </c>
-      <c r="D40" s="32">
+      <c r="D40" s="30">
         <v>0.98160919540229796</v>
       </c>
       <c r="E40" s="20">
@@ -2435,7 +3113,16 @@
       <c r="H40" s="4">
         <v>3.6296496498445699E-2</v>
       </c>
-      <c r="K40" s="6"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
@@ -2469,13 +3156,13 @@
       <c r="A41" s="16">
         <v>25</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="32">
+      <c r="C41" s="30">
         <v>0.65739910313901295</v>
       </c>
-      <c r="D41" s="32">
+      <c r="D41" s="30">
         <v>0.433183856502242</v>
       </c>
       <c r="E41" s="20">
@@ -2490,7 +3177,16 @@
       <c r="H41" s="4">
         <v>5.7536764751762497E-2</v>
       </c>
-      <c r="K41" s="6"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
@@ -2524,13 +3220,13 @@
       <c r="A42" s="16">
         <v>29</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="32">
+      <c r="C42" s="30">
         <v>0.96984435797665303</v>
       </c>
-      <c r="D42" s="32">
+      <c r="D42" s="30">
         <v>0.96498054474708095</v>
       </c>
       <c r="E42" s="20">
@@ -2545,7 +3241,16 @@
       <c r="H42" s="4">
         <v>1.7097556811478499E-2</v>
       </c>
-      <c r="K42" s="6"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
@@ -2579,13 +3284,13 @@
       <c r="A43" s="16">
         <v>31</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="32">
+      <c r="C43" s="30">
         <v>0.93545858374706004</v>
       </c>
-      <c r="D43" s="32">
+      <c r="D43" s="30">
         <v>0.93467467990593101</v>
       </c>
       <c r="E43" s="20">
@@ -2600,7 +3305,16 @@
       <c r="H43" s="4">
         <v>6.6991737155132805E-2</v>
       </c>
-      <c r="K43" s="6"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
@@ -2634,11 +3348,11 @@
       <c r="A44" s="16">
         <v>35</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="20"/>
       <c r="F44" s="20">
         <v>7.8737010391686596E-2</v>
@@ -2649,7 +3363,16 @@
       <c r="H44" s="4">
         <v>4.2580027810611099E-2</v>
       </c>
-      <c r="K44" s="6"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
@@ -2683,11 +3406,11 @@
       <c r="A45" s="16">
         <v>50</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="20">
         <v>0.19220549158547301</v>
       </c>
@@ -2700,6 +3423,16 @@
       <c r="H45" s="4">
         <v>0.282002348237679</v>
       </c>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
       <c r="U45" s="5"/>
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
@@ -2754,6 +3487,16 @@
       <c r="H46" s="4">
         <v>0.10077749367633</v>
       </c>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
@@ -2784,6 +3527,16 @@
       <c r="AV46" s="5"/>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
@@ -2820,6 +3573,16 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
       <c r="U48" s="5"/>
       <c r="V48" s="5"/>
       <c r="W48" s="5"/>
@@ -2858,7 +3621,7 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="28"/>
+      <c r="G49" s="26"/>
       <c r="U49" s="5"/>
       <c r="V49" s="5"/>
       <c r="W49" s="5"/>
@@ -2889,17 +3652,17 @@
       <c r="AV49" s="5"/>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="37" t="s">
+      <c r="B50" s="37"/>
+      <c r="C50" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="38"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="40"/>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
       <c r="W50" s="5"/>
@@ -2931,7 +3694,7 @@
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A51" s="15"/>
-      <c r="B51" s="29"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="10">
         <v>10</v>
       </c>
@@ -2983,13 +3746,13 @@
       <c r="A52" s="16">
         <v>3</v>
       </c>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="32">
+      <c r="C52" s="30">
         <v>3.3663484627932998E-2</v>
       </c>
-      <c r="D52" s="32">
+      <c r="D52" s="30">
         <v>3.3663484627932998E-2</v>
       </c>
       <c r="E52" s="20">
@@ -2998,7 +3761,7 @@
       <c r="F52" s="20">
         <v>0.76806582627279796</v>
       </c>
-      <c r="G52" s="34">
+      <c r="G52" s="32">
         <v>0.81749132245336797</v>
       </c>
       <c r="H52" s="4">
@@ -3037,13 +3800,13 @@
       <c r="A53" s="16">
         <v>4</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="32">
+      <c r="C53" s="30">
         <v>2.4819394918706401E-2</v>
       </c>
-      <c r="D53" s="32">
+      <c r="D53" s="30">
         <v>3.4871404322187702E-2</v>
       </c>
       <c r="E53" s="20">
@@ -3052,7 +3815,7 @@
       <c r="F53" s="20">
         <v>0.62215680477975999</v>
       </c>
-      <c r="G53" s="34">
+      <c r="G53" s="32">
         <v>0.71106110837018199</v>
       </c>
       <c r="H53" s="4">
@@ -3091,13 +3854,13 @@
       <c r="A54" s="16">
         <v>5</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C54" s="10">
         <v>0.88686594456960199</v>
       </c>
-      <c r="D54" s="32">
+      <c r="D54" s="30">
         <v>0.88686594456960199</v>
       </c>
       <c r="E54" s="20">
@@ -3145,13 +3908,13 @@
       <c r="A55" s="16">
         <v>7</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C55" s="30">
         <v>0.29202651134766</v>
       </c>
-      <c r="D55" s="32">
+      <c r="D55" s="30">
         <v>0.499501182296816</v>
       </c>
       <c r="E55" s="20">
@@ -3160,7 +3923,7 @@
       <c r="F55" s="20">
         <v>0.94062463966264098</v>
       </c>
-      <c r="G55" s="34">
+      <c r="G55" s="32">
         <v>0.97205060311856395</v>
       </c>
       <c r="H55" s="4">
@@ -3199,13 +3962,13 @@
       <c r="A56" s="16">
         <v>16</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="32">
+      <c r="C56" s="30">
         <v>0.90593453129427703</v>
       </c>
-      <c r="D56" s="32">
+      <c r="D56" s="30">
         <v>0.92243907848169004</v>
       </c>
       <c r="E56" s="19">
@@ -3253,13 +4016,13 @@
       <c r="A57" s="16">
         <v>17</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="32">
+      <c r="C57" s="30">
         <v>0.97570754226844203</v>
       </c>
-      <c r="D57" s="32">
+      <c r="D57" s="30">
         <v>0.98885015423683598</v>
       </c>
       <c r="E57" s="20">
@@ -3268,7 +4031,7 @@
       <c r="F57" s="19">
         <v>0.99007733884190396</v>
       </c>
-      <c r="G57" s="36">
+      <c r="G57" s="34">
         <v>0.98978899095279604</v>
       </c>
       <c r="H57" s="4">
@@ -3307,13 +4070,13 @@
       <c r="A58" s="16">
         <v>18</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="32">
+      <c r="C58" s="30">
         <v>0.89266075217515095</v>
       </c>
-      <c r="D58" s="32">
+      <c r="D58" s="30">
         <v>0.90478512862104499</v>
       </c>
       <c r="E58" s="20">
@@ -3361,13 +4124,13 @@
       <c r="A59" s="16">
         <v>19</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="32">
+      <c r="C59" s="30">
         <v>0.93435239349876997</v>
       </c>
-      <c r="D59" s="32">
+      <c r="D59" s="30">
         <v>0.94828551173463604</v>
       </c>
       <c r="E59" s="19">
@@ -3415,13 +4178,13 @@
       <c r="A60" s="16">
         <v>20</v>
       </c>
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="32">
+      <c r="C60" s="30">
         <v>0.79105832109969298</v>
       </c>
-      <c r="D60" s="32">
+      <c r="D60" s="30">
         <v>0.88585846731604201</v>
       </c>
       <c r="E60" s="19">
@@ -3469,13 +4232,13 @@
       <c r="A61" s="16">
         <v>21</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="32">
+      <c r="C61" s="30">
         <v>0.94161515292717102</v>
       </c>
-      <c r="D61" s="32">
+      <c r="D61" s="30">
         <v>0.96034598192355602</v>
       </c>
       <c r="E61" s="20">
@@ -3523,13 +4286,13 @@
       <c r="A62" s="16">
         <v>22</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="32">
+      <c r="C62" s="30">
         <v>0.95439384255813098</v>
       </c>
-      <c r="D62" s="32">
+      <c r="D62" s="30">
         <v>0.96680356735873096</v>
       </c>
       <c r="E62" s="20">
@@ -3577,13 +4340,13 @@
       <c r="A63" s="16">
         <v>25</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="10">
         <v>0.64564613434259999</v>
       </c>
-      <c r="D63" s="32">
+      <c r="D63" s="30">
         <v>0.53389061365424495</v>
       </c>
       <c r="E63" s="20">
@@ -3631,13 +4394,13 @@
       <c r="A64" s="16">
         <v>29</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="32">
+      <c r="C64" s="30">
         <v>0.74485938482625702</v>
       </c>
-      <c r="D64" s="32">
+      <c r="D64" s="30">
         <v>0.88918398512714902</v>
       </c>
       <c r="E64" s="19">
@@ -3674,13 +4437,13 @@
       <c r="A65" s="16">
         <v>31</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="32">
+      <c r="C65" s="30">
         <v>9.4603009607656094E-2</v>
       </c>
-      <c r="D65" s="32">
+      <c r="D65" s="30">
         <v>0.140529372502293</v>
       </c>
       <c r="E65" s="20">
@@ -3689,7 +4452,7 @@
       <c r="F65" s="20">
         <v>0.85262157632272295</v>
       </c>
-      <c r="G65" s="34">
+      <c r="G65" s="32">
         <v>0.8808354443702</v>
       </c>
       <c r="H65" s="4">
@@ -3717,11 +4480,11 @@
       <c r="A66" s="16">
         <v>35</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="20"/>
       <c r="F66" s="19">
         <v>1.15362092523911E-2</v>
@@ -3754,18 +4517,18 @@
       <c r="A67" s="16">
         <v>50</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="20">
         <v>0.168058226350488</v>
       </c>
       <c r="F67" s="20">
         <v>0.37428333460305502</v>
       </c>
-      <c r="G67" s="34">
+      <c r="G67" s="32">
         <v>0.42209156560767502</v>
       </c>
       <c r="H67" s="4">
@@ -3802,7 +4565,7 @@
       <c r="D68" s="8">
         <v>0.61949542216291098</v>
       </c>
-      <c r="E68" s="35">
+      <c r="E68" s="33">
         <v>0.66499926245762198</v>
       </c>
       <c r="F68" s="22">
@@ -3860,7 +4623,7 @@
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="28"/>
+      <c r="G70" s="26"/>
       <c r="V70" s="5"/>
       <c r="W70" s="5"/>
       <c r="X70" s="5"/>
@@ -3880,17 +4643,17 @@
       <c r="AL70" s="5"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B71" s="40"/>
-      <c r="C71" s="37" t="s">
+      <c r="B71" s="37"/>
+      <c r="C71" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="38"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="40"/>
       <c r="V71" s="5"/>
       <c r="W71" s="5"/>
       <c r="X71" s="5"/>
@@ -3911,7 +4674,7 @@
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
-      <c r="B72" s="29"/>
+      <c r="B72" s="27"/>
       <c r="C72" s="10">
         <v>10</v>
       </c>
@@ -3952,13 +4715,13 @@
       <c r="A73" s="16">
         <v>3</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="32">
+      <c r="C73" s="30">
         <v>3.7929419645764601E-3</v>
       </c>
-      <c r="D73" s="32">
+      <c r="D73" s="30">
         <v>3.7929419645764601E-3</v>
       </c>
       <c r="E73" s="20">
@@ -3995,13 +4758,13 @@
       <c r="A74" s="16">
         <v>4</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="32">
+      <c r="C74" s="30">
         <v>2.22870828578691E-3</v>
       </c>
-      <c r="D74" s="32">
+      <c r="D74" s="30">
         <v>3.1822188744333501E-3</v>
       </c>
       <c r="E74" s="20">
@@ -4038,13 +4801,13 @@
       <c r="A75" s="16">
         <v>5</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C75" s="32">
+      <c r="C75" s="30">
         <v>0.38892233594220299</v>
       </c>
-      <c r="D75" s="32">
+      <c r="D75" s="30">
         <v>0.38892233594220299</v>
       </c>
       <c r="E75" s="20">
@@ -4081,13 +4844,13 @@
       <c r="A76" s="16">
         <v>7</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B76" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="32">
+      <c r="C76" s="30">
         <v>2.2483537158984001E-2</v>
       </c>
-      <c r="D76" s="32">
+      <c r="D76" s="30">
         <v>7.3529411764705802E-2</v>
       </c>
       <c r="E76" s="20">
@@ -4107,13 +4870,13 @@
       <c r="A77" s="16">
         <v>16</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="32">
+      <c r="C77" s="30">
         <v>0.424648049849988</v>
       </c>
-      <c r="D77" s="32">
+      <c r="D77" s="30">
         <v>0.48391420911528099</v>
       </c>
       <c r="E77" s="20">
@@ -4133,13 +4896,13 @@
       <c r="A78" s="16">
         <v>17</v>
       </c>
-      <c r="B78" s="30" t="s">
+      <c r="B78" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="32">
+      <c r="C78" s="30">
         <v>0.636640704368438</v>
       </c>
-      <c r="D78" s="32">
+      <c r="D78" s="30">
         <v>0.665371024734982</v>
       </c>
       <c r="E78" s="20">
@@ -4159,13 +4922,13 @@
       <c r="A79" s="16">
         <v>18</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="32">
+      <c r="C79" s="30">
         <v>0.61695906432748504</v>
       </c>
-      <c r="D79" s="32">
+      <c r="D79" s="30">
         <v>0.61234567901234505</v>
       </c>
       <c r="E79" s="20">
@@ -4185,13 +4948,13 @@
       <c r="A80" s="16">
         <v>19</v>
       </c>
-      <c r="B80" s="30" t="s">
+      <c r="B80" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C80" s="32">
+      <c r="C80" s="30">
         <v>0.73989755264655599</v>
       </c>
-      <c r="D80" s="32">
+      <c r="D80" s="30">
         <v>0.80755176613885504</v>
       </c>
       <c r="E80" s="20">
@@ -4211,13 +4974,13 @@
       <c r="A81" s="16">
         <v>20</v>
       </c>
-      <c r="B81" s="30" t="s">
+      <c r="B81" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C81" s="32">
+      <c r="C81" s="30">
         <v>0.41573033707865098</v>
       </c>
-      <c r="D81" s="32">
+      <c r="D81" s="30">
         <v>0.784037558685446</v>
       </c>
       <c r="E81" s="20">
@@ -4237,13 +5000,13 @@
       <c r="A82" s="16">
         <v>21</v>
       </c>
-      <c r="B82" s="30" t="s">
+      <c r="B82" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="32">
+      <c r="C82" s="30">
         <v>0.57875428662572703</v>
       </c>
-      <c r="D82" s="32">
+      <c r="D82" s="30">
         <v>0.624882749211222</v>
       </c>
       <c r="E82" s="20">
@@ -4263,13 +5026,13 @@
       <c r="A83" s="16">
         <v>22</v>
       </c>
-      <c r="B83" s="30" t="s">
+      <c r="B83" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C83" s="32">
+      <c r="C83" s="30">
         <v>0.62749181791133501</v>
       </c>
-      <c r="D83" s="32">
+      <c r="D83" s="30">
         <v>0.63109665976943496</v>
       </c>
       <c r="E83" s="20">
@@ -4289,13 +5052,13 @@
       <c r="A84" s="16">
         <v>25</v>
       </c>
-      <c r="B84" s="30" t="s">
+      <c r="B84" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="32">
+      <c r="C84" s="30">
         <v>0.33872458410351203</v>
       </c>
-      <c r="D84" s="32">
+      <c r="D84" s="30">
         <v>0.31014554794520499</v>
       </c>
       <c r="E84" s="20">
@@ -4315,13 +5078,13 @@
       <c r="A85" s="16">
         <v>29</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="32">
+      <c r="C85" s="30">
         <v>0.17033999658294799</v>
       </c>
-      <c r="D85" s="32">
+      <c r="D85" s="30">
         <v>0.28820453224869202</v>
       </c>
       <c r="E85" s="20">
@@ -4341,13 +5104,13 @@
       <c r="A86" s="16">
         <v>31</v>
       </c>
-      <c r="B86" s="30" t="s">
+      <c r="B86" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C86" s="32">
+      <c r="C86" s="30">
         <v>1.81621709374825E-2</v>
       </c>
-      <c r="D86" s="32">
+      <c r="D86" s="30">
         <v>3.1972612780106699E-2</v>
       </c>
       <c r="E86" s="20">
@@ -4367,11 +5130,11 @@
       <c r="A87" s="16">
         <v>35</v>
       </c>
-      <c r="B87" s="30" t="s">
+      <c r="B87" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
       <c r="E87" s="20"/>
       <c r="F87" s="20">
         <v>8.0483719410058396E-3</v>
@@ -4387,11 +5150,11 @@
       <c r="A88" s="16">
         <v>50</v>
       </c>
-      <c r="B88" s="30" t="s">
+      <c r="B88" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
       <c r="E88" s="20">
         <v>8.0048482293423207E-2</v>
       </c>
@@ -4432,18 +5195,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:Q28"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AC23:AD23"/>
     <mergeCell ref="AE23:AF23"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>